<commit_message>
update to LCA module
</commit_message>
<xml_diff>
--- a/LCC/rals_livslangd_python/data/raw/LCA/LCC assessment - indata.xlsx
+++ b/LCC/rals_livslangd_python/data/raw/LCA/LCC assessment - indata.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtioffice365.sharepoint.com/sites/Underhllstabeller/Delade dokument/General/AP4/LCCA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdouAA\Work Folders\Documents\GitHub\rurut\LCC\rals_livslangd_python\data\raw\LCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1102" documentId="13_ncr:1_{0E8D36DC-5EAF-491F-9C74-C89F8723C50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CEEAECA-BD20-4EC3-9555-C39F9F0872D2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331D07F8-F689-4FCF-83F5-C1413CD638D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-1980" windowWidth="29016" windowHeight="18216" firstSheet="1" activeTab="2" xr2:uid="{A0E77FEA-D435-4ED7-B278-0D20F96847F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{A0E77FEA-D435-4ED7-B278-0D20F96847F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
     <sheet name="LCC indata" sheetId="4" r:id="rId2"/>
-    <sheet name="LCA indata_EF" sheetId="9" r:id="rId3"/>
-    <sheet name="LCA calculation" sheetId="12" r:id="rId4"/>
-    <sheet name="LCC calculation" sheetId="3" r:id="rId5"/>
-    <sheet name="Train disturbance parameters" sheetId="5" r:id="rId6"/>
-    <sheet name="Method info." sheetId="1" r:id="rId7"/>
-    <sheet name="CO2_Valuation" sheetId="10" r:id="rId8"/>
-    <sheet name="Energy use emission factors" sheetId="11" r:id="rId9"/>
+    <sheet name="LCA indata_EF_CSV" sheetId="13" r:id="rId3"/>
+    <sheet name="LCA indata_EF" sheetId="9" r:id="rId4"/>
+    <sheet name="LCA calculation" sheetId="12" r:id="rId5"/>
+    <sheet name="LCC calculation" sheetId="3" r:id="rId6"/>
+    <sheet name="Train disturbance parameters" sheetId="5" r:id="rId7"/>
+    <sheet name="Method info." sheetId="1" r:id="rId8"/>
+    <sheet name="CO2_Valuation" sheetId="10" r:id="rId9"/>
+    <sheet name="Energy use emission factors" sheetId="11" r:id="rId10"/>
+    <sheet name="Energy use emission factors_CSV" sheetId="14" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_Ref103090875" localSheetId="4">'LCC calculation'!#REF!</definedName>
+    <definedName name="_Ref103090875" localSheetId="5">'LCC calculation'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="337">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1238,6 +1240,18 @@
   </si>
   <si>
     <t>Social costs, Reinvestment / year (SEK/m)</t>
+  </si>
+  <si>
+    <t>Quantity (in meter)</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>What</t>
+  </si>
+  <si>
+    <t>Track</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2173,7 @@
     <xf numFmtId="43" fontId="53" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="53" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="251">
+  <cellXfs count="250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2675,6 +2689,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2687,26 +2717,9 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6010,10 +6023,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 – 2022">
   <a:themeElements>
@@ -6704,6 +6713,630 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FC3526-9AC2-46EA-B815-EC7FCC78A064}">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" t="s">
+        <v>305</v>
+      </c>
+      <c r="L1" t="s">
+        <v>315</v>
+      </c>
+      <c r="M1" t="s">
+        <v>316</v>
+      </c>
+      <c r="N1" t="s">
+        <v>317</v>
+      </c>
+      <c r="O1" t="s">
+        <v>318</v>
+      </c>
+      <c r="P1" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>320</v>
+      </c>
+      <c r="R1" t="s">
+        <v>327</v>
+      </c>
+      <c r="S1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f xml:space="preserve"> 100 - A2</f>
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <f>A2*$R$2 + B2*$R$3</f>
+        <v>0.64649243466299866</v>
+      </c>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="L2" t="s">
+        <v>321</v>
+      </c>
+      <c r="M2">
+        <v>2020</v>
+      </c>
+      <c r="N2">
+        <v>43.25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>322</v>
+      </c>
+      <c r="P2">
+        <v>2.75</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>323</v>
+      </c>
+      <c r="R2">
+        <f>P2/N2</f>
+        <v>6.358381502890173E-2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+5</f>
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0" xml:space="preserve"> 100 - A3</f>
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C22" si="1">A3*$R$2 + B3*$R$3</f>
+        <v>0.93208688807435736</v>
+      </c>
+      <c r="G3" s="231"/>
+      <c r="H3" s="231"/>
+      <c r="I3" s="231"/>
+      <c r="L3" t="s">
+        <v>325</v>
+      </c>
+      <c r="M3">
+        <v>2020</v>
+      </c>
+      <c r="N3">
+        <v>7.27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>326</v>
+      </c>
+      <c r="P3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>324</v>
+      </c>
+      <c r="R3">
+        <f>P3/N3</f>
+        <v>6.4649243466299864E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A22" si="2">A3+5</f>
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>1.2176813414857162</v>
+      </c>
+      <c r="G4" s="231"/>
+      <c r="H4" s="231"/>
+      <c r="I4" s="231"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>1.5032757948970747</v>
+      </c>
+      <c r="G5" s="231"/>
+      <c r="H5" s="231"/>
+      <c r="I5" s="231"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1.7888702483084336</v>
+      </c>
+      <c r="G6" s="231"/>
+      <c r="H6" s="231"/>
+      <c r="I6" s="231"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>2.0744647017197924</v>
+      </c>
+      <c r="G7" s="231"/>
+      <c r="H7" s="231"/>
+      <c r="I7" s="231"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>2.3600591551311507</v>
+      </c>
+      <c r="G8" s="231"/>
+      <c r="H8" s="231"/>
+      <c r="I8" s="231"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>2.64565360854251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>2.9312480619538688</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>3.2168425153652267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>3.5024369687765855</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>3.7880314221879443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>4.0736258755993031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>4.3592203290106619</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>4.6448147824220207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>4.9304092358333795</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>5.2160036892447383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>5.5015981426560971</v>
+      </c>
+      <c r="L19" s="230"/>
+      <c r="M19" s="230"/>
+      <c r="N19" s="230"/>
+      <c r="O19" s="230"/>
+      <c r="P19" s="230"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>5.7871925960674551</v>
+      </c>
+      <c r="L20" s="231"/>
+      <c r="M20" s="231"/>
+      <c r="N20" s="231"/>
+      <c r="O20" s="231"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>6.0727870494788148</v>
+      </c>
+      <c r="L21" s="231"/>
+      <c r="M21" s="231"/>
+      <c r="N21" s="231"/>
+      <c r="O21" s="231"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>6.3583815028901727</v>
+      </c>
+      <c r="L22" s="231"/>
+      <c r="M22" s="231"/>
+      <c r="N22" s="231"/>
+      <c r="O22" s="231"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L23" s="231"/>
+      <c r="M23" s="231"/>
+      <c r="N23" s="231"/>
+      <c r="O23" s="231"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L24" s="231"/>
+      <c r="M24" s="231"/>
+      <c r="N24" s="231"/>
+      <c r="O24" s="231"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L25" s="231"/>
+      <c r="M25" s="231"/>
+      <c r="N25" s="231"/>
+      <c r="O25" s="231"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C98BF6-34EB-407A-8213-9F60BB33BDE4}">
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="C2">
+        <v>43.25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E2">
+        <v>2.75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G2">
+        <f>E2/C2</f>
+        <v>6.358381502890173E-2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+      <c r="C3">
+        <v>7.27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G3">
+        <f>E3/C3</f>
+        <v>6.4649243466299864E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="231"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D5" s="231"/>
+      <c r="E5" s="231"/>
+      <c r="F5" s="231"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D6" s="231"/>
+      <c r="E6" s="231"/>
+      <c r="F6" s="231"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D7" s="231"/>
+      <c r="E7" s="231"/>
+      <c r="F7" s="231"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="231"/>
+    </row>
+    <row r="19" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I19" s="230"/>
+      <c r="J19" s="230"/>
+      <c r="K19" s="230"/>
+      <c r="L19" s="230"/>
+      <c r="M19" s="230"/>
+    </row>
+    <row r="20" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I20" s="231"/>
+      <c r="J20" s="231"/>
+      <c r="K20" s="231"/>
+      <c r="L20" s="231"/>
+    </row>
+    <row r="21" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I21" s="231"/>
+      <c r="J21" s="231"/>
+      <c r="K21" s="231"/>
+      <c r="L21" s="231"/>
+    </row>
+    <row r="22" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I22" s="231"/>
+      <c r="J22" s="231"/>
+      <c r="K22" s="231"/>
+      <c r="L22" s="231"/>
+    </row>
+    <row r="23" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I23" s="231"/>
+      <c r="J23" s="231"/>
+      <c r="K23" s="231"/>
+      <c r="L23" s="231"/>
+    </row>
+    <row r="24" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I24" s="231"/>
+      <c r="J24" s="231"/>
+      <c r="K24" s="231"/>
+      <c r="L24" s="231"/>
+    </row>
+    <row r="25" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I25" s="231"/>
+      <c r="J25" s="231"/>
+      <c r="K25" s="231"/>
+      <c r="L25" s="231"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDF281D-924C-4FA2-981E-BBF25D33068E}">
   <dimension ref="A1:G52"/>
@@ -7441,11 +8074,326 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80E84EE-2883-4F3A-8EB4-7732CB32E152}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" s="232" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" s="232" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1" s="232" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1" s="232" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" s="232" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="233" t="s">
+        <v>290</v>
+      </c>
+      <c r="H1" s="233" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2">
+        <f>467.3950042*1000</f>
+        <v>467395.00420000002</v>
+      </c>
+      <c r="F2">
+        <v>4752.6315249999998</v>
+      </c>
+      <c r="G2" t="s">
+        <v>291</v>
+      </c>
+      <c r="H2" s="236" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E3" s="240">
+        <f>9.347900083*1000</f>
+        <v>9347.9000830000004</v>
+      </c>
+      <c r="F3">
+        <v>95.05263051</v>
+      </c>
+      <c r="G3" t="s">
+        <v>291</v>
+      </c>
+      <c r="H3" t="s">
+        <v>292</v>
+      </c>
+      <c r="I3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E4">
+        <f>0.717088628*1000</f>
+        <v>717.08862799999997</v>
+      </c>
+      <c r="F4">
+        <v>141.21226329999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E5">
+        <f>329.8885214*1000</f>
+        <v>329888.52140000003</v>
+      </c>
+      <c r="F5">
+        <v>3040.2167679999998</v>
+      </c>
+      <c r="G5" t="s">
+        <v>291</v>
+      </c>
+      <c r="H5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E6" s="239">
+        <f>6.597770427*1000</f>
+        <v>6597.7704270000004</v>
+      </c>
+      <c r="F6">
+        <v>60.804335360000003</v>
+      </c>
+      <c r="G6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>298</v>
+      </c>
+      <c r="E7" s="55">
+        <f>15.94567051*1000</f>
+        <v>15945.67051</v>
+      </c>
+      <c r="F7" s="55">
+        <v>155.85696590000001</v>
+      </c>
+      <c r="G7" t="s">
+        <v>274</v>
+      </c>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" s="55">
+        <f>0.717088628*1000</f>
+        <v>717.08862799999997</v>
+      </c>
+      <c r="F8" s="55">
+        <v>141.21226329999999</v>
+      </c>
+      <c r="G8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>283</v>
+      </c>
+      <c r="E9" s="55">
+        <f>0.66687297*1000</f>
+        <v>666.87297000000001</v>
+      </c>
+      <c r="F9" s="55">
+        <v>10.19917369</v>
+      </c>
+      <c r="G9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>315</v>
+      </c>
+      <c r="B11" t="s">
+        <v>316</v>
+      </c>
+      <c r="C11" t="s">
+        <v>317</v>
+      </c>
+      <c r="D11" t="s">
+        <v>318</v>
+      </c>
+      <c r="E11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F11" t="s">
+        <v>320</v>
+      </c>
+      <c r="G11" t="s">
+        <v>327</v>
+      </c>
+      <c r="H11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12">
+        <v>43.25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E12">
+        <v>2.75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>323</v>
+      </c>
+      <c r="G12">
+        <f>E12/C12</f>
+        <v>6.358381502890173E-2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>325</v>
+      </c>
+      <c r="B13">
+        <v>2020</v>
+      </c>
+      <c r="C13">
+        <v>7.27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>326</v>
+      </c>
+      <c r="E13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>324</v>
+      </c>
+      <c r="G13">
+        <f>E13/C13</f>
+        <v>6.4649243466299864E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A1FB41-4712-42FA-A521-99FFF6F99586}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7539,7 +8487,7 @@
         <f>F2*H2</f>
         <v>3072.54032565337</v>
       </c>
-      <c r="J2" s="250">
+      <c r="J2" s="241">
         <f>LOOKUP(CO2_Valuation!A8, CO2_Valuation!A:A, CO2_Valuation!B:B)</f>
         <v>2.2237799999999996</v>
       </c>
@@ -7571,7 +8519,7 @@
       <c r="D3" t="s">
         <v>286</v>
       </c>
-      <c r="E3" s="249">
+      <c r="E3" s="240">
         <f>9.347900083*1000</f>
         <v>9347.9000830000004</v>
       </c>
@@ -7590,7 +8538,7 @@
         <f>F3*H3</f>
         <v>88.920076572080234</v>
       </c>
-      <c r="J3" s="250">
+      <c r="J3" s="241">
         <f>LOOKUP(CO2_Valuation!A8, CO2_Valuation!A:A, CO2_Valuation!B:B)</f>
         <v>2.2237799999999996</v>
       </c>
@@ -7598,7 +8546,7 @@
         <f>LOOKUP(CO2_Valuation!A9, CO2_Valuation!A:A, CO2_Valuation!B:B)*(E3+I3)*1000</f>
         <v>22312511.953493815</v>
       </c>
-      <c r="L3" s="249">
+      <c r="L3" s="240">
         <f t="shared" ref="L3:L6" si="0">K3/1000</f>
         <v>22312.511953493817</v>
       </c>
@@ -7644,7 +8592,7 @@
         <f>F4*H4</f>
         <v>168.87761071844034</v>
       </c>
-      <c r="J4" s="250">
+      <c r="J4" s="241">
         <f>LOOKUP(CO2_Valuation!A8, CO2_Valuation!A:A, CO2_Valuation!B:B)</f>
         <v>2.2237799999999996</v>
       </c>
@@ -7680,7 +8628,7 @@
       <c r="F5">
         <v>3040.2167679999998</v>
       </c>
-      <c r="G5" s="246">
+      <c r="G5" s="237">
         <f>'Energy use emission factors'!A10</f>
         <v>40</v>
       </c>
@@ -7692,7 +8640,7 @@
         <f>F5*H5</f>
         <v>4340.7741519884221</v>
       </c>
-      <c r="J5" s="250">
+      <c r="J5" s="241">
         <f>LOOKUP(CO2_Valuation!A8, CO2_Valuation!A:A, CO2_Valuation!B:B)</f>
         <v>2.2237799999999996</v>
       </c>
@@ -7724,7 +8672,7 @@
       <c r="D6" t="s">
         <v>286</v>
       </c>
-      <c r="E6" s="248">
+      <c r="E6" s="239">
         <f>6.597770427*1000</f>
         <v>6597.7704270000004</v>
       </c>
@@ -7743,7 +8691,7 @@
         <f>F6*H6</f>
         <v>99.177720266937982</v>
       </c>
-      <c r="J6" s="250">
+      <c r="J6" s="241">
         <f>LOOKUP(CO2_Valuation!A8, CO2_Valuation!A:A, CO2_Valuation!B:B)</f>
         <v>2.2237799999999996</v>
       </c>
@@ -7751,7 +8699,7 @@
         <f>LOOKUP(CO2_Valuation!A12, CO2_Valuation!A:A, CO2_Valuation!B:B)*(E6+I6)*1000</f>
         <v>18659706.622729871</v>
       </c>
-      <c r="L6" s="248">
+      <c r="L6" s="239">
         <f t="shared" si="0"/>
         <v>18659.706622729871</v>
       </c>
@@ -7774,7 +8722,7 @@
         <v>155.85696590000001</v>
       </c>
       <c r="G7" s="235"/>
-      <c r="J7" s="250"/>
+      <c r="J7" s="241"/>
       <c r="M7" t="s">
         <v>274</v>
       </c>
@@ -7795,7 +8743,7 @@
         <v>141.21226329999999</v>
       </c>
       <c r="G8" s="235"/>
-      <c r="J8" s="250"/>
+      <c r="J8" s="241"/>
       <c r="M8" t="s">
         <v>274</v>
       </c>
@@ -7815,7 +8763,7 @@
         <v>10.19917369</v>
       </c>
       <c r="G9" s="235"/>
-      <c r="J9" s="250"/>
+      <c r="J9" s="241"/>
       <c r="M9" t="s">
         <v>274</v>
       </c>
@@ -7827,35 +8775,35 @@
       <c r="N10" s="55"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="245" t="s">
+      <c r="A11" t="s">
         <v>295</v>
       </c>
       <c r="B11" t="s">
         <v>307</v>
       </c>
-      <c r="D11" s="245" t="s">
+      <c r="D11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="245" t="s">
+      <c r="A12" t="s">
         <v>296</v>
       </c>
-      <c r="D12" s="245" t="s">
+      <c r="D12" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="245" t="s">
+      <c r="A13" t="s">
         <v>297</v>
       </c>
-      <c r="D13" s="245" t="s">
+      <c r="D13" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E15" s="247"/>
-      <c r="F15" s="247"/>
+      <c r="E15" s="238"/>
+      <c r="F15" s="238"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -7863,7 +8811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AC1756-7DB9-46B2-B62B-0BC8C4179448}">
   <dimension ref="A1:G103"/>
   <sheetViews>
@@ -7881,16 +8829,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="117"/>
-      <c r="B1" s="241" t="s">
+      <c r="B1" s="242" t="s">
         <v>332</v>
       </c>
-      <c r="C1" s="242"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="241" t="s">
+      <c r="C1" s="243"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="242" t="s">
         <v>310</v>
       </c>
-      <c r="F1" s="242"/>
-      <c r="G1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="244"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="120" t="s">
@@ -9242,7 +10190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07E81E6-84A4-4797-A70A-3EF8DC212FF3}">
   <dimension ref="A1:BF107"/>
   <sheetViews>
@@ -9384,37 +10332,37 @@
       <c r="AH2" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="237" t="s">
+      <c r="AI2" s="245" t="s">
         <v>14</v>
       </c>
-      <c r="AJ2" s="237"/>
-      <c r="AK2" s="237"/>
-      <c r="AL2" s="237" t="s">
+      <c r="AJ2" s="245"/>
+      <c r="AK2" s="245"/>
+      <c r="AL2" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="AM2" s="237"/>
-      <c r="AN2" s="237"/>
-      <c r="AO2" s="237"/>
-      <c r="AP2" s="237"/>
-      <c r="AQ2" s="237"/>
+      <c r="AM2" s="245"/>
+      <c r="AN2" s="245"/>
+      <c r="AO2" s="245"/>
+      <c r="AP2" s="245"/>
+      <c r="AQ2" s="245"/>
       <c r="AR2" s="84"/>
       <c r="AS2" s="84"/>
-      <c r="AT2" s="237" t="s">
+      <c r="AT2" s="245" t="s">
         <v>16</v>
       </c>
-      <c r="AU2" s="237"/>
-      <c r="AV2" s="237"/>
-      <c r="AW2" s="237" t="s">
+      <c r="AU2" s="245"/>
+      <c r="AV2" s="245"/>
+      <c r="AW2" s="245" t="s">
         <v>17</v>
       </c>
-      <c r="AX2" s="237"/>
-      <c r="AY2" s="237"/>
-      <c r="AZ2" s="237"/>
-      <c r="BA2" s="237"/>
-      <c r="BB2" s="237"/>
-      <c r="BC2" s="237"/>
-      <c r="BD2" s="237"/>
-      <c r="BE2" s="237"/>
+      <c r="AX2" s="245"/>
+      <c r="AY2" s="245"/>
+      <c r="AZ2" s="245"/>
+      <c r="BA2" s="245"/>
+      <c r="BB2" s="245"/>
+      <c r="BC2" s="245"/>
+      <c r="BD2" s="245"/>
+      <c r="BE2" s="245"/>
     </row>
     <row r="3" spans="1:58" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="67"/>
@@ -9572,71 +10520,71 @@
       </c>
       <c r="P5" s="146"/>
       <c r="R5" s="117"/>
-      <c r="S5" s="241" t="s">
+      <c r="S5" s="242" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="242"/>
-      <c r="U5" s="243"/>
-      <c r="V5" s="241" t="s">
+      <c r="T5" s="243"/>
+      <c r="U5" s="244"/>
+      <c r="V5" s="242" t="s">
         <v>15</v>
       </c>
-      <c r="W5" s="242"/>
-      <c r="X5" s="243"/>
+      <c r="W5" s="243"/>
+      <c r="X5" s="244"/>
       <c r="Y5" s="85"/>
       <c r="Z5" s="117"/>
-      <c r="AA5" s="241" t="s">
+      <c r="AA5" s="242" t="s">
         <v>16</v>
       </c>
-      <c r="AB5" s="242"/>
-      <c r="AC5" s="243"/>
-      <c r="AD5" s="241" t="s">
+      <c r="AB5" s="243"/>
+      <c r="AC5" s="244"/>
+      <c r="AD5" s="242" t="s">
         <v>27</v>
       </c>
-      <c r="AE5" s="242"/>
-      <c r="AF5" s="243"/>
+      <c r="AE5" s="243"/>
+      <c r="AF5" s="244"/>
       <c r="AG5" s="84"/>
       <c r="AH5" s="121"/>
-      <c r="AI5" s="238" t="str">
+      <c r="AI5" s="246" t="str">
         <f>C19</f>
         <v>Rail renewal (material + work)</v>
       </c>
-      <c r="AJ5" s="239"/>
-      <c r="AK5" s="240"/>
-      <c r="AL5" s="238" t="str">
+      <c r="AJ5" s="247"/>
+      <c r="AK5" s="248"/>
+      <c r="AL5" s="246" t="str">
         <f>C22</f>
         <v>Disposal of rail waste (neg. value if benefit)</v>
       </c>
-      <c r="AM5" s="239"/>
-      <c r="AN5" s="240"/>
-      <c r="AO5" s="238" t="str">
+      <c r="AM5" s="247"/>
+      <c r="AN5" s="248"/>
+      <c r="AO5" s="246" t="str">
         <f>C16</f>
         <v>Residual (remaining service life of rail)</v>
       </c>
-      <c r="AP5" s="239"/>
-      <c r="AQ5" s="240"/>
+      <c r="AP5" s="247"/>
+      <c r="AQ5" s="248"/>
       <c r="AR5" s="84"/>
       <c r="AS5" s="121"/>
-      <c r="AT5" s="238" t="str">
+      <c r="AT5" s="246" t="str">
         <f>C20</f>
         <v>Grinding</v>
       </c>
-      <c r="AU5" s="239"/>
-      <c r="AV5" s="240"/>
-      <c r="AW5" s="238" t="s">
+      <c r="AU5" s="247"/>
+      <c r="AV5" s="248"/>
+      <c r="AW5" s="246" t="s">
         <v>28</v>
       </c>
-      <c r="AX5" s="239"/>
-      <c r="AY5" s="239"/>
-      <c r="AZ5" s="239" t="s">
+      <c r="AX5" s="247"/>
+      <c r="AY5" s="247"/>
+      <c r="AZ5" s="247" t="s">
         <v>29</v>
       </c>
-      <c r="BA5" s="239"/>
-      <c r="BB5" s="239"/>
-      <c r="BC5" s="239" t="s">
+      <c r="BA5" s="247"/>
+      <c r="BB5" s="247"/>
+      <c r="BC5" s="247" t="s">
         <v>29</v>
       </c>
-      <c r="BD5" s="239"/>
-      <c r="BE5" s="240"/>
+      <c r="BD5" s="247"/>
+      <c r="BE5" s="248"/>
       <c r="BF5" s="1"/>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.3">
@@ -27281,12 +28229,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="AD5:AF5"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="AI5:AK5"/>
     <mergeCell ref="AL2:AQ2"/>
     <mergeCell ref="AW5:AY5"/>
     <mergeCell ref="AZ5:BB5"/>
@@ -27296,6 +28238,12 @@
     <mergeCell ref="AT5:AV5"/>
     <mergeCell ref="AL5:AN5"/>
     <mergeCell ref="AO5:AQ5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="AD5:AF5"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="AI5:AK5"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27304,7 +28252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758EE40C-7333-432E-9E7E-B3CEB4915EE7}">
   <dimension ref="A2:I26"/>
   <sheetViews>
@@ -27329,17 +28277,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C2" s="244" t="s">
+      <c r="C2" s="249" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244" t="s">
+      <c r="D2" s="249"/>
+      <c r="E2" s="249"/>
+      <c r="F2" s="249"/>
+      <c r="G2" s="249" t="s">
         <v>150</v>
       </c>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
+      <c r="H2" s="249"/>
+      <c r="I2" s="249"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -27990,7 +28938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8C7FA3-4D8F-416A-8180-3F1712469FB5}">
   <dimension ref="B1:R25"/>
   <sheetViews>
@@ -28446,7 +29394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722AAB82-8796-4A9E-80EE-A1455E7CB9A2}">
   <dimension ref="A1:C38"/>
   <sheetViews>
@@ -28772,461 +29720,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FC3526-9AC2-46EA-B815-EC7FCC78A064}">
-  <dimension ref="A1:S25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C1" t="s">
-        <v>305</v>
-      </c>
-      <c r="L1" t="s">
-        <v>315</v>
-      </c>
-      <c r="M1" t="s">
-        <v>316</v>
-      </c>
-      <c r="N1" t="s">
-        <v>317</v>
-      </c>
-      <c r="O1" t="s">
-        <v>318</v>
-      </c>
-      <c r="P1" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>320</v>
-      </c>
-      <c r="R1" t="s">
-        <v>327</v>
-      </c>
-      <c r="S1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f xml:space="preserve"> 100 - A2</f>
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <f>A2*$R$2 + B2*$R$3</f>
-        <v>0.64649243466299866</v>
-      </c>
-      <c r="G2" s="230"/>
-      <c r="H2" s="230"/>
-      <c r="L2" t="s">
-        <v>321</v>
-      </c>
-      <c r="M2">
-        <v>2020</v>
-      </c>
-      <c r="N2">
-        <v>43.25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>322</v>
-      </c>
-      <c r="P2">
-        <v>2.75</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>323</v>
-      </c>
-      <c r="R2">
-        <f>P2/N2</f>
-        <v>6.358381502890173E-2</v>
-      </c>
-      <c r="S2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <f>A2+5</f>
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B22" si="0" xml:space="preserve"> 100 - A3</f>
-        <v>95</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C32" si="1">A3*$R$2 + B3*$R$3</f>
-        <v>0.93208688807435736</v>
-      </c>
-      <c r="G3" s="231"/>
-      <c r="H3" s="231"/>
-      <c r="I3" s="231"/>
-      <c r="L3" t="s">
-        <v>325</v>
-      </c>
-      <c r="M3">
-        <v>2020</v>
-      </c>
-      <c r="N3">
-        <v>7.27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>326</v>
-      </c>
-      <c r="P3">
-        <v>4.7E-2</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>324</v>
-      </c>
-      <c r="R3">
-        <f>P3/N3</f>
-        <v>6.4649243466299864E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <f t="shared" ref="A4:A25" si="2">A3+5</f>
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
-        <v>1.2176813414857162</v>
-      </c>
-      <c r="G4" s="231"/>
-      <c r="H4" s="231"/>
-      <c r="I4" s="231"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
-        <v>1.5032757948970747</v>
-      </c>
-      <c r="G5" s="231"/>
-      <c r="H5" s="231"/>
-      <c r="I5" s="231"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
-        <v>1.7888702483084336</v>
-      </c>
-      <c r="G6" s="231"/>
-      <c r="H6" s="231"/>
-      <c r="I6" s="231"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>2.0744647017197924</v>
-      </c>
-      <c r="G7" s="231"/>
-      <c r="H7" s="231"/>
-      <c r="I7" s="231"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>2.3600591551311507</v>
-      </c>
-      <c r="G8" s="231"/>
-      <c r="H8" s="231"/>
-      <c r="I8" s="231"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
-        <v>2.64565360854251</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
-        <v>2.9312480619538688</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>3.2168425153652267</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>3.5024369687765855</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>3.7880314221879443</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>4.0736258755993031</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="2"/>
-        <v>65</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>4.3592203290106619</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>4.6448147824220207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>4.9304092358333795</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="2"/>
-        <v>80</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>5.2160036892447383</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>5.5015981426560971</v>
-      </c>
-      <c r="L19" s="230"/>
-      <c r="M19" s="230"/>
-      <c r="N19" s="230"/>
-      <c r="O19" s="230"/>
-      <c r="P19" s="230"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>5.7871925960674551</v>
-      </c>
-      <c r="L20" s="231"/>
-      <c r="M20" s="231"/>
-      <c r="N20" s="231"/>
-      <c r="O20" s="231"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f t="shared" si="2"/>
-        <v>95</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>6.0727870494788148</v>
-      </c>
-      <c r="L21" s="231"/>
-      <c r="M21" s="231"/>
-      <c r="N21" s="231"/>
-      <c r="O21" s="231"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
-        <v>6.3583815028901727</v>
-      </c>
-      <c r="L22" s="231"/>
-      <c r="M22" s="231"/>
-      <c r="N22" s="231"/>
-      <c r="O22" s="231"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="L23" s="231"/>
-      <c r="M23" s="231"/>
-      <c r="N23" s="231"/>
-      <c r="O23" s="231"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="L24" s="231"/>
-      <c r="M24" s="231"/>
-      <c r="N24" s="231"/>
-      <c r="O24" s="231"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="L25" s="231"/>
-      <c r="M25" s="231"/>
-      <c r="N25" s="231"/>
-      <c r="O25" s="231"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -29237,17 +29730,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75ec815d-4f26-4607-8475-2e9d903770b6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51def2a5-4310-4eb1-8e7f-d05231fbe784" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100E0BBAAF5B6E7334E92AD404531F7A6F7" ma:contentTypeVersion="11" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="5d2b631ed35b6fabae17b34a6dae9174">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="75ec815d-4f26-4607-8475-2e9d903770b6" xmlns:ns3="51def2a5-4310-4eb1-8e7f-d05231fbe784" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64ef8f22ee785b675903b1d9127d0dec" ns2:_="" ns3:_="">
     <xsd:import namespace="75ec815d-4f26-4607-8475-2e9d903770b6"/>
@@ -29442,6 +29924,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75ec815d-4f26-4607-8475-2e9d903770b6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51def2a5-4310-4eb1-8e7f-d05231fbe784" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B3C93BF-01B0-466E-A306-5B8BE5A5F096}">
   <ds:schemaRefs>
@@ -29451,24 +29944,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668E4520-06CC-4635-8D30-EB65F6359CAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="90c39dbe-e643-451f-b686-8821d465838f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="75ec815d-4f26-4607-8475-2e9d903770b6"/>
-    <ds:schemaRef ds:uri="51def2a5-4310-4eb1-8e7f-d05231fbe784"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8579EA1F-78CD-4C87-87E2-FE39016AD4AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29485,4 +29960,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668E4520-06CC-4635-8D30-EB65F6359CAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="90c39dbe-e643-451f-b686-8821d465838f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="75ec815d-4f26-4607-8475-2e9d903770b6"/>
+    <ds:schemaRef ds:uri="51def2a5-4310-4eb1-8e7f-d05231fbe784"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>